<commit_message>
AH | fix some excel template
</commit_message>
<xml_diff>
--- a/application/download/pws_template/template_pws_ibu1.xlsx
+++ b/application/download/pws_template/template_pws_ibu1.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\dho\application\download\pws_template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="396" yWindow="552" windowWidth="19812" windowHeight="7368"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -379,20 +384,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -402,6 +393,20 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,6 +416,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -706,25 +714,25 @@
   </sheetPr>
   <dimension ref="A1:AMK71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:F35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.3984375" style="38" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="8.09765625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="38" customWidth="1"/>
-    <col min="6" max="11" width="11.69921875" style="38" customWidth="1"/>
-    <col min="12" max="13" width="12.796875" style="1" customWidth="1"/>
-    <col min="14" max="20" width="12.796875" style="38" customWidth="1"/>
-    <col min="21" max="30" width="26.09765625" style="38" customWidth="1"/>
-    <col min="31" max="1025" width="11.69921875" style="38" customWidth="1"/>
+    <col min="1" max="1" width="5.3828125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="21.61328125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" style="38" customWidth="1"/>
+    <col min="4" max="4" width="8.07421875" style="38" customWidth="1"/>
+    <col min="5" max="5" width="10.61328125" style="38" customWidth="1"/>
+    <col min="6" max="11" width="11.69140625" style="38" customWidth="1"/>
+    <col min="12" max="13" width="12.765625" style="1" customWidth="1"/>
+    <col min="14" max="20" width="12.765625" style="38" customWidth="1"/>
+    <col min="21" max="30" width="26.07421875" style="38" customWidth="1"/>
+    <col min="31" max="1025" width="11.69140625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -760,7 +768,7 @@
       <c r="AC1" s="8"/>
       <c r="AD1" s="8"/>
     </row>
-    <row r="2" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -794,7 +802,7 @@
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
     </row>
-    <row r="3" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -828,7 +836,7 @@
       <c r="AC3" s="8"/>
       <c r="AD3" s="8"/>
     </row>
-    <row r="4" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -862,7 +870,7 @@
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
     </row>
-    <row r="5" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -896,7 +904,7 @@
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
     </row>
-    <row r="6" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -928,39 +936,39 @@
       <c r="AC6" s="8"/>
       <c r="AD6" s="8"/>
     </row>
-    <row r="7" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+    <row r="7" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="47" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="47" t="s">
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="47" t="s">
+      <c r="M7" s="51"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -972,57 +980,57 @@
       <c r="AC7" s="8"/>
       <c r="AD7" s="8"/>
     </row>
-    <row r="8" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49" t="s">
+    <row r="8" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="48"/>
-      <c r="L8" s="47" t="s">
+      <c r="K8" s="49"/>
+      <c r="L8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="47" t="s">
+      <c r="M8" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="47" t="s">
+      <c r="N8" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="49" t="s">
+      <c r="O8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="47" t="s">
+      <c r="P8" s="49"/>
+      <c r="Q8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="47" t="s">
+      <c r="R8" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="49" t="s">
+      <c r="S8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="48"/>
+      <c r="T8" s="49"/>
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
@@ -1034,33 +1042,33 @@
       <c r="AC8" s="8"/>
       <c r="AD8" s="8"/>
     </row>
-    <row r="9" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+    <row r="9" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="18" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="48"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="49"/>
       <c r="O9" s="18" t="s">
         <v>20</v>
       </c>
       <c r="P9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
       <c r="S9" s="18" t="s">
         <v>20</v>
       </c>
@@ -1078,7 +1086,7 @@
       <c r="AC9" s="8"/>
       <c r="AD9" s="8"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="41">
         <v>1</v>
       </c>
@@ -1148,7 +1156,7 @@
       <c r="AC10" s="8"/>
       <c r="AD10" s="8"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -1198,7 +1206,7 @@
       <c r="AC11" s="8"/>
       <c r="AD11" s="8"/>
     </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -1248,7 +1256,7 @@
       <c r="AC12" s="8"/>
       <c r="AD12" s="8"/>
     </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -1298,7 +1306,7 @@
       <c r="AC13" s="8"/>
       <c r="AD13" s="8"/>
     </row>
-    <row r="14" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -1348,7 +1356,7 @@
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
     </row>
-    <row r="15" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -1398,7 +1406,7 @@
       <c r="AC15" s="8"/>
       <c r="AD15" s="8"/>
     </row>
-    <row r="16" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -1448,7 +1456,7 @@
       <c r="AC16" s="8"/>
       <c r="AD16" s="8"/>
     </row>
-    <row r="17" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1498,7 +1506,7 @@
       <c r="AC17" s="8"/>
       <c r="AD17" s="8"/>
     </row>
-    <row r="18" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1548,7 +1556,7 @@
       <c r="AC18" s="8"/>
       <c r="AD18" s="8"/>
     </row>
-    <row r="19" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1598,7 +1606,7 @@
       <c r="AC19" s="8"/>
       <c r="AD19" s="8"/>
     </row>
-    <row r="20" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1648,7 +1656,7 @@
       <c r="AC20" s="8"/>
       <c r="AD20" s="8"/>
     </row>
-    <row r="21" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1698,7 +1706,7 @@
       <c r="AC21" s="8"/>
       <c r="AD21" s="8"/>
     </row>
-    <row r="22" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="19" t="s">
         <v>22</v>
@@ -1750,7 +1758,7 @@
       <c r="AC22" s="8"/>
       <c r="AD22" s="8"/>
     </row>
-    <row r="23" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="19" t="s">
         <v>22</v>
@@ -1802,15 +1810,15 @@
       <c r="AC23" s="8"/>
       <c r="AD23" s="8"/>
     </row>
-    <row r="24" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
+    <row r="24" spans="1:30" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="47"/>
       <c r="B24" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
@@ -1854,7 +1862,7 @@
       <c r="AC24" s="8"/>
       <c r="AD24" s="8"/>
     </row>
-    <row r="25" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -1904,7 +1912,7 @@
       <c r="AC25" s="8"/>
       <c r="AD25" s="8"/>
     </row>
-    <row r="26" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -1954,7 +1962,7 @@
       <c r="AC26" s="8"/>
       <c r="AD26" s="8"/>
     </row>
-    <row r="27" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -2004,7 +2012,7 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="8"/>
     </row>
-    <row r="28" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -2054,7 +2062,7 @@
       <c r="AC28" s="8"/>
       <c r="AD28" s="8"/>
     </row>
-    <row r="29" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -2104,7 +2112,7 @@
       <c r="AC29" s="8"/>
       <c r="AD29" s="8"/>
     </row>
-    <row r="30" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -2154,7 +2162,7 @@
       <c r="AC30" s="8"/>
       <c r="AD30" s="8"/>
     </row>
-    <row r="31" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -2204,7 +2212,7 @@
       <c r="AC31" s="8"/>
       <c r="AD31" s="8"/>
     </row>
-    <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -2254,7 +2262,7 @@
       <c r="AC32" s="8"/>
       <c r="AD32" s="8"/>
     </row>
-    <row r="33" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="19" t="s">
         <v>22</v>
@@ -2306,7 +2314,7 @@
       <c r="AC33" s="8"/>
       <c r="AD33" s="8"/>
     </row>
-    <row r="34" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="19" t="s">
         <v>22</v>
@@ -2358,15 +2366,15 @@
       <c r="AC34" s="8"/>
       <c r="AD34" s="8"/>
     </row>
-    <row r="35" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51"/>
-      <c r="B35" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
+    <row r="35" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="45"/>
+      <c r="B35" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
@@ -2410,11 +2418,11 @@
       <c r="AC35" s="8"/>
       <c r="AD35" s="8"/>
     </row>
-    <row r="36" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="45" t="s">
+    <row r="36" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="46"/>
+      <c r="B36" s="53"/>
       <c r="C36" s="40">
         <f t="shared" ref="C36:I36" si="12">SUM(C11:C35)</f>
         <v>0</v>
@@ -2498,7 +2506,7 @@
       <c r="AC36" s="8"/>
       <c r="AD36" s="8"/>
     </row>
-    <row r="37" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24"/>
       <c r="B37" s="25" t="s">
         <v>22</v>
@@ -2532,7 +2540,7 @@
       <c r="AC37" s="8"/>
       <c r="AD37" s="8"/>
     </row>
-    <row r="38" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="31"/>
       <c r="B38" s="11" t="s">
         <v>22</v>
@@ -2568,7 +2576,7 @@
       <c r="AC38" s="8"/>
       <c r="AD38" s="8"/>
     </row>
-    <row r="39" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="31"/>
       <c r="B39" s="11" t="s">
         <v>22</v>
@@ -2604,7 +2612,7 @@
       <c r="AC39" s="8"/>
       <c r="AD39" s="8"/>
     </row>
-    <row r="40" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="31"/>
       <c r="B40" s="11" t="s">
         <v>22</v>
@@ -2638,7 +2646,7 @@
       <c r="AC40" s="8"/>
       <c r="AD40" s="8"/>
     </row>
-    <row r="41" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31"/>
       <c r="B41" s="11" t="s">
         <v>22</v>
@@ -2672,7 +2680,7 @@
       <c r="AC41" s="8"/>
       <c r="AD41" s="8"/>
     </row>
-    <row r="42" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="31"/>
       <c r="B42" s="11" t="s">
         <v>22</v>
@@ -2708,7 +2716,7 @@
       <c r="AC42" s="8"/>
       <c r="AD42" s="8"/>
     </row>
-    <row r="43" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="B43" s="15" t="s">
         <v>22</v>
@@ -2744,154 +2752,148 @@
       <c r="AC43" s="8"/>
       <c r="AD43" s="8"/>
     </row>
-    <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="38" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:P7"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="Q7:T7"/>
     <mergeCell ref="C8:C9"/>
@@ -2908,6 +2910,12 @@
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:P7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>